<commit_message>
fix: leitura do config.txt e caminho base ajustado para C:\sistemaRemessas\modelos
</commit_message>
<xml_diff>
--- a/modelos/fichas.xlsx
+++ b/modelos/fichas.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr codeName="EstaPasta_de_trabalho" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leandro.sobrinho\Desktop\sistemaRemessas\modelos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sistemaRemessas\modelos\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E629197C-153B-458F-A1ED-B012DF967373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dados" sheetId="1" r:id="rId1"/>
@@ -99,7 +100,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="\R&quot;R$&quot;\ #,##0.00"/>
@@ -166,7 +167,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -195,6 +196,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="22" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -216,9 +220,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -256,9 +260,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -293,7 +297,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -328,7 +332,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -501,12 +505,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Planilha1"/>
   <dimension ref="A1:AC33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="Z14" sqref="Z14"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -614,8 +618,11 @@
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="F2" s="4"/>
       <c r="I2" s="5"/>
+      <c r="K2" s="9"/>
+      <c r="M2" s="9"/>
       <c r="P2" s="5"/>
       <c r="Q2" s="4"/>
+      <c r="X2" s="10"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="F3" s="4"/>
@@ -736,7 +743,7 @@
       <c r="AC33" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="pSwnuNIQn4FHtaMS/TTOAtplyi8Fa4qFSzvimlliHCx90XSfFGt12mLVQg76tNrdfVF21L3DVyQ0oimVnpJo3Q==" saltValue="w2GGeFUiUNu29uvYsiYMag==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="I80HsefsW6AEso55PMXTQNvu9XI0g7jW5CNNHG2II/aLHYsIyN/YDa88C5w/Bxs8QILMFyKK6b0vgWuZeq4M1Q==" saltValue="DDweNr0b1bHSg2/NqLCKYw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
FIX: Adaptado o caminho de config para fichaFormulario e tbm Modelo de Remessa
</commit_message>
<xml_diff>
--- a/modelos/fichas.xlsx
+++ b/modelos/fichas.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sistemaRemessas\modelos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E629197C-153B-458F-A1ED-B012DF967373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6485EF6-1CA3-43F6-9171-3AA2A2DEF830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dados" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t>Paciente</t>
   </si>
@@ -95,6 +108,51 @@
   </si>
   <si>
     <t>Responsavel</t>
+  </si>
+  <si>
+    <t>Leandro Sobrinho Auzier</t>
+  </si>
+  <si>
+    <t>Ciclano de tal</t>
+  </si>
+  <si>
+    <t>HCAL</t>
+  </si>
+  <si>
+    <t>EX: 123/2500</t>
+  </si>
+  <si>
+    <t>Neurologia</t>
+  </si>
+  <si>
+    <t>000000.0000.0000.0454/2025</t>
+  </si>
+  <si>
+    <t>Não</t>
+  </si>
+  <si>
+    <t>Sim</t>
+  </si>
+  <si>
+    <t>Fulano Credor de tal</t>
+  </si>
+  <si>
+    <t>9699999-9999</t>
+  </si>
+  <si>
+    <t>000.000.000-33</t>
+  </si>
+  <si>
+    <t>banco do brasil</t>
+  </si>
+  <si>
+    <t>0000-0</t>
+  </si>
+  <si>
+    <t>Nome do Responsável</t>
+  </si>
+  <si>
+    <t>01/02/1200</t>
   </si>
 </sst>
 </file>
@@ -167,7 +225,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -199,6 +257,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="22" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -616,13 +677,81 @@
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="F2" s="4"/>
-      <c r="I2" s="5"/>
-      <c r="K2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="4"/>
-      <c r="X2" s="10"/>
+      <c r="A2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="5">
+        <v>45658</v>
+      </c>
+      <c r="J2" s="3">
+        <v>5</v>
+      </c>
+      <c r="K2" s="9">
+        <v>24.75</v>
+      </c>
+      <c r="L2" s="3">
+        <v>2</v>
+      </c>
+      <c r="M2" s="9">
+        <v>247.5</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="P2" s="5">
+        <v>45658</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="R2" s="3">
+        <v>0</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="X2" s="10">
+        <v>46002.541875000003</v>
+      </c>
+      <c r="Y2" s="11">
+        <v>46002.556956018518</v>
+      </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="F3" s="4"/>
@@ -743,7 +872,7 @@
       <c r="AC33" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="I80HsefsW6AEso55PMXTQNvu9XI0g7jW5CNNHG2II/aLHYsIyN/YDa88C5w/Bxs8QILMFyKK6b0vgWuZeq4M1Q==" saltValue="DDweNr0b1bHSg2/NqLCKYw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="oBv0x4jF9D1nFVshBn+FuDzepNQYENrilVjMjVNmhDsQ6DtrlqSPuf5swXdlE6yJp83QDjj6+qs/g96G3wou+g==" saltValue="gYube/ZW47jVc7DTGyESnA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" sort="0" autoFilter="0" selectUnlockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Ajuste na limpeza de dados vcazios na remessa
</commit_message>
<xml_diff>
--- a/modelos/fichas.xlsx
+++ b/modelos/fichas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sistemaRemessas\modelos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6485EF6-1CA3-43F6-9171-3AA2A2DEF830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20FF5B8B-48B9-4A74-832C-2B7A76EC526C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Paciente</t>
   </si>
@@ -108,51 +108,6 @@
   </si>
   <si>
     <t>Responsavel</t>
-  </si>
-  <si>
-    <t>Leandro Sobrinho Auzier</t>
-  </si>
-  <si>
-    <t>Ciclano de tal</t>
-  </si>
-  <si>
-    <t>HCAL</t>
-  </si>
-  <si>
-    <t>EX: 123/2500</t>
-  </si>
-  <si>
-    <t>Neurologia</t>
-  </si>
-  <si>
-    <t>000000.0000.0000.0454/2025</t>
-  </si>
-  <si>
-    <t>Não</t>
-  </si>
-  <si>
-    <t>Sim</t>
-  </si>
-  <si>
-    <t>Fulano Credor de tal</t>
-  </si>
-  <si>
-    <t>9699999-9999</t>
-  </si>
-  <si>
-    <t>000.000.000-33</t>
-  </si>
-  <si>
-    <t>banco do brasil</t>
-  </si>
-  <si>
-    <t>0000-0</t>
-  </si>
-  <si>
-    <t>Nome do Responsável</t>
-  </si>
-  <si>
-    <t>01/02/1200</t>
   </si>
 </sst>
 </file>
@@ -570,8 +525,8 @@
   <sheetPr codeName="Planilha1"/>
   <dimension ref="A1:AC33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="Z21" sqref="Z21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -677,87 +632,24 @@
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="I2" s="5">
-        <v>45658</v>
-      </c>
-      <c r="J2" s="3">
-        <v>5</v>
-      </c>
-      <c r="K2" s="9">
-        <v>24.75</v>
-      </c>
-      <c r="L2" s="3">
-        <v>2</v>
-      </c>
-      <c r="M2" s="9">
-        <v>247.5</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="P2" s="5">
-        <v>45658</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="R2" s="3">
-        <v>0</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="X2" s="10">
-        <v>46002.541875000003</v>
-      </c>
-      <c r="Y2" s="11">
-        <v>46002.556956018518</v>
-      </c>
+      <c r="F2" s="4"/>
+      <c r="I2" s="5"/>
+      <c r="K2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="4"/>
+      <c r="X2" s="10"/>
+      <c r="Y2" s="11"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="F3" s="4"/>
       <c r="I3" s="5"/>
+      <c r="K3" s="9"/>
+      <c r="M3" s="9"/>
       <c r="P3" s="5"/>
       <c r="Q3" s="4"/>
+      <c r="X3" s="10"/>
+      <c r="Y3" s="11"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="F4" s="4"/>
@@ -872,7 +764,7 @@
       <c r="AC33" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="oBv0x4jF9D1nFVshBn+FuDzepNQYENrilVjMjVNmhDsQ6DtrlqSPuf5swXdlE6yJp83QDjj6+qs/g96G3wou+g==" saltValue="gYube/ZW47jVc7DTGyESnA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" sort="0" autoFilter="0" selectUnlockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="TYz1nr1xoGgWebtD5/6gXl/jo2k5IBwfJMgCcDtITFlYMEA9FFuyha5rbTDnKVKLUQg7DpvoDH5hYgtpBgtepQ==" saltValue="6oTXxVNlTudpaPc9S4HzWQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
FIX: Ajustado os campos Destino e período da planilha modelo de Remessas e linhas serão apagadas em caso de não houver mais dados para preencher a cópia gerada
</commit_message>
<xml_diff>
--- a/modelos/fichas.xlsx
+++ b/modelos/fichas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sistemaRemessas\modelos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20FF5B8B-48B9-4A74-832C-2B7A76EC526C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA6D7DE3-179A-4774-B62D-DBD5C694AA79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dados" sheetId="1" r:id="rId1"/>
@@ -526,7 +526,7 @@
   <dimension ref="A1:AC33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="Z21" sqref="Z21"/>
+      <selection activeCell="Y10" sqref="Y10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -764,7 +764,7 @@
       <c r="AC33" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="TYz1nr1xoGgWebtD5/6gXl/jo2k5IBwfJMgCcDtITFlYMEA9FFuyha5rbTDnKVKLUQg7DpvoDH5hYgtpBgtepQ==" saltValue="6oTXxVNlTudpaPc9S4HzWQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="ckNXhJ07HS4dYa/7p7OkBZawl6JDpvdrUoQP7Wf2Kq08wR0AYCxEK1EvNeMYVdKJoJoQ/HZSscyXfOoeEOSjbw==" saltValue="mAkziJ5Hdc6kzdDwxdbZXw==" spinCount="100000" sheet="1" objects="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Editado docm removendo botoes e paginas em branco do documento e limpeza dos dados na planilha fichas
</commit_message>
<xml_diff>
--- a/modelos/fichas.xlsx
+++ b/modelos/fichas.xlsx
@@ -1,34 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr codeName="EstaPasta_de_trabalho" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sistemaRemessas\modelos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA6D7DE3-179A-4774-B62D-DBD5C694AA79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Dados" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -113,11 +99,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="\R&quot;R$&quot;\ #,##0.00"/>
-    <numFmt numFmtId="166" formatCode="&quot;R$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="165" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -180,7 +165,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -206,9 +191,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="22" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -236,9 +218,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -276,9 +258,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -313,7 +295,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -348,7 +330,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -521,12 +503,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Planilha1"/>
   <dimension ref="A1:AC33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="Y10" sqref="Y10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -634,26 +616,28 @@
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="F2" s="4"/>
       <c r="I2" s="5"/>
-      <c r="K2" s="9"/>
-      <c r="M2" s="9"/>
+      <c r="K2" s="8"/>
+      <c r="M2" s="8"/>
       <c r="P2" s="5"/>
       <c r="Q2" s="4"/>
-      <c r="X2" s="10"/>
-      <c r="Y2" s="11"/>
+      <c r="X2" s="9"/>
+      <c r="Y2" s="10"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="F3" s="4"/>
       <c r="I3" s="5"/>
-      <c r="K3" s="9"/>
-      <c r="M3" s="9"/>
+      <c r="K3" s="8"/>
+      <c r="M3" s="8"/>
       <c r="P3" s="5"/>
       <c r="Q3" s="4"/>
-      <c r="X3" s="10"/>
-      <c r="Y3" s="11"/>
+      <c r="X3" s="9"/>
+      <c r="Y3" s="10"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="F4" s="4"/>
       <c r="I4" s="5"/>
+      <c r="K4" s="8"/>
+      <c r="M4" s="8"/>
       <c r="P4" s="5"/>
       <c r="Q4" s="4"/>
     </row>
@@ -668,34 +652,40 @@
     <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="F6" s="4"/>
       <c r="I6" s="5"/>
-      <c r="K6" s="9"/>
-      <c r="M6" s="9"/>
+      <c r="K6" s="8"/>
+      <c r="M6" s="8"/>
       <c r="P6" s="5"/>
       <c r="Q6" s="4"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="F7" s="4"/>
       <c r="I7" s="5"/>
-      <c r="K7" s="9"/>
-      <c r="M7" s="9"/>
+      <c r="K7" s="8"/>
+      <c r="M7" s="8"/>
       <c r="P7" s="5"/>
       <c r="Q7" s="4"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="F8" s="4"/>
       <c r="I8" s="5"/>
+      <c r="K8" s="8"/>
+      <c r="M8" s="8"/>
       <c r="P8" s="5"/>
       <c r="Q8" s="4"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="F9" s="4"/>
       <c r="I9" s="5"/>
+      <c r="K9" s="8"/>
+      <c r="M9" s="8"/>
       <c r="P9" s="5"/>
       <c r="Q9" s="4"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="F10" s="4"/>
       <c r="I10" s="5"/>
+      <c r="K10" s="8"/>
+      <c r="M10" s="8"/>
       <c r="P10" s="5"/>
       <c r="Q10" s="4"/>
     </row>
@@ -764,7 +754,7 @@
       <c r="AC33" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="ckNXhJ07HS4dYa/7p7OkBZawl6JDpvdrUoQP7Wf2Kq08wR0AYCxEK1EvNeMYVdKJoJoQ/HZSscyXfOoeEOSjbw==" saltValue="mAkziJ5Hdc6kzdDwxdbZXw==" spinCount="100000" sheet="1" objects="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="oTVXQpuQeC1DISKi0nM4TB1u5c1vKBlJUfdnX+H+Z7NGN7WgR139cuSIjqBcVg4XNGTdxfruVF5Zh/ilEDlpIQ==" saltValue="h2H+QP8El70N5LK9K5K5aQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualização de emissão de remessas
</commit_message>
<xml_diff>
--- a/modelos/fichas.xlsx
+++ b/modelos/fichas.xlsx
@@ -507,8 +507,8 @@
   <sheetPr codeName="Planilha1"/>
   <dimension ref="A1:AC33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AA9" sqref="AA9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -754,7 +754,7 @@
       <c r="AC33" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="oTVXQpuQeC1DISKi0nM4TB1u5c1vKBlJUfdnX+H+Z7NGN7WgR139cuSIjqBcVg4XNGTdxfruVF5Zh/ilEDlpIQ==" saltValue="h2H+QP8El70N5LK9K5K5aQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="iPsjCZ3iGSfDX+Aot1ACDQfXfPfp9u7sBAnfW6+s6YLqgbW0Ogq06HTEAnluOEHrbJeAEfXWE8BZaI6A2dwf+Q==" saltValue="bFjvQRXNpuasHFPLj46PgA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>